<commit_message>
moved .xlsx files from src/test to /test_
</commit_message>
<xml_diff>
--- a/test_cases/SimpleArrayDict.xlsx
+++ b/test_cases/SimpleArrayDict.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_16AB0E5D1BC4BC2CF2998C16798A565729086C1E" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7B143FE3-4F1A-7049-AEA1-64A142517942}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="2" r:id="rId1"/>
@@ -127,15 +126,15 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>C:\Users\thangiswho\Desktop\uipath_AutomationTestRobot\src\test\SimpleArrayDict.xaml</t>
+    <t>C:\Users\rpa-dev\Desktop\FPT-Thang\ロボソース\AutomationTestRobot\test\SimpleArrayDict.xaml</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,7 +263,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="標準 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -541,23 +540,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56" style="7" customWidth="1"/>
-    <col min="3" max="3" width="59.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="59.375" style="4" customWidth="1"/>
     <col min="4" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="38">
+    <row r="2" spans="1:3" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -577,67 +576,67 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
@@ -650,7 +649,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -658,20 +657,20 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="33" style="4" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.875" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="59.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="13.75" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.25" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59.375" style="4" customWidth="1"/>
     <col min="9" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -697,7 +696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -715,7 +714,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
@@ -733,7 +732,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
@@ -751,7 +750,7 @@
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
         <v>18</v>
       </c>
@@ -769,7 +768,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
@@ -787,7 +786,7 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="8" t="s">
         <v>22</v>
       </c>
@@ -805,7 +804,7 @@
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -823,7 +822,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -833,7 +832,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -843,7 +842,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -853,7 +852,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -863,7 +862,7 @@
       <c r="G12" s="6"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -876,7 +875,7 @@
   </sheetData>
   <phoneticPr fontId="4"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>"In,Out"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>